<commit_message>
Adding final changes to repo
</commit_message>
<xml_diff>
--- a/Docs/Tarea5-6/TP-DES.xlsx
+++ b/Docs/Tarea5-6/TP-DES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49b8cc00b261ecde/JP/TEC/MAESTRIA/IV_Cuatri/Verificacion y Validacion de Software/Tarea5-6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicsma2409\Desktop\Maestria\1er Cuatrimestre 2025\Verificacion\ProyectoFinal\Repo_SSH\Docs\Tarea5-6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{586B33B5-572F-4504-800E-3514601EE4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEC6EC7C-B2C3-4641-81E4-3A5E3A36EDC8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A17D07-C034-4F19-99D2-1755071AB680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caso de Prueba" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -282,9 +282,6 @@
     <t>Para desactivar los sensores, darle click a todos los botones hasta que esten en color gris</t>
   </si>
   <si>
-    <t>Para activar los sensores, darle click a todos los botones ahsta que esten en color rojo</t>
-  </si>
-  <si>
     <t>Verificar que el indicador "Bocina" se encuentra encendido (Color Rojo) debido a la activación del Sensor S2</t>
   </si>
   <si>
@@ -327,9 +324,6 @@
     <t>Verificar que el indicador "ALERTA: S2" se encuentra Apagado (Color Rojo) debido al cambio de modo a Desarmado</t>
   </si>
   <si>
-    <t>Verificar que al activar todos los sensores el es Modo Activo es  "DESARMADO"</t>
-  </si>
-  <si>
     <t>TP-DES-002</t>
   </si>
   <si>
@@ -343,6 +337,16 @@
   </si>
   <si>
     <t>Verificación de caso cuando se cambia de modo a desarmado</t>
+  </si>
+  <si>
+    <t>Para activar los sensores, darle click a todos los botones hasta que esten en color rojo</t>
+  </si>
+  <si>
+    <t>Verificar que al activar todos los sensores el Modo Activo es  "DESARMADO"</t>
+  </si>
+  <si>
+    <t>SW-ID-65
+SW-ID-66</t>
   </si>
 </sst>
 </file>
@@ -937,11 +941,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
@@ -1134,13 +1138,13 @@
     </row>
     <row r="13" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>50</v>
@@ -1155,7 +1159,7 @@
         <v>60</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>43</v>
@@ -1175,13 +1179,13 @@
     </row>
     <row r="14" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>50</v>
@@ -1196,7 +1200,7 @@
         <v>60</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>43</v>
@@ -1212,13 +1216,13 @@
     </row>
     <row r="15" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>50</v>
@@ -1233,7 +1237,7 @@
         <v>60</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>43</v>
@@ -1249,16 +1253,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="F9:L9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:L10"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B9:B11"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="F9:L9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:L10"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
@@ -1278,11 +1282,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="56.7109375" customWidth="1"/>
@@ -1526,7 +1530,7 @@
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="13" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1535,7 +1539,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>80</v>
@@ -1601,11 +1605,11 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
-        <f t="shared" si="0"/>
+        <f>1+A24</f>
         <v>13</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>43</v>
@@ -1615,7 +1619,7 @@
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1624,7 +1628,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>43</v>
@@ -1641,7 +1645,7 @@
         <v>15</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
         <v>43</v>
@@ -1658,7 +1662,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1671,10 +1675,10 @@
         <v>17</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>71</v>
@@ -1690,7 +1694,7 @@
         <v>18</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>43</v>
@@ -1700,7 +1704,7 @@
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1741,7 +1745,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>43</v>
@@ -1751,7 +1755,7 @@
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1760,7 +1764,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>43</v>
@@ -1777,7 +1781,7 @@
         <v>23</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>43</v>
@@ -1787,7 +1791,7 @@
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1796,7 +1800,7 @@
         <v>24</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1809,10 +1813,10 @@
         <v>25</v>
       </c>
       <c r="B37" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>98</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>66</v>
@@ -1831,7 +1835,7 @@
         <v>70</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>71</v>
@@ -1843,7 +1847,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E38" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pasó, Falló"</formula1>
     </dataValidation>

</xml_diff>